<commit_message>
Update the sprint1 backlog,modify the product backlog&Requirements Outline.
</commit_message>
<xml_diff>
--- a/documents/product backlog.xlsx
+++ b/documents/product backlog.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="90" windowWidth="19200" windowHeight="11640"/>
@@ -11,7 +11,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -55,11 +55,6 @@
     <t>Release 2</t>
   </si>
   <si>
-    <t xml:space="preserve">
-show  elegant demeanor of assistants</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>An assistant manages his/her own basic  information and working information</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -128,29 +123,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <r>
-      <t>design the index of the website(</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>首页</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>)</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Effort in the whole backlog</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -173,13 +145,21 @@
   <si>
     <t>lrx</t>
     <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>show  elegant demeanor of assistants</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>design the home page of the website</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="10">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -230,12 +210,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="204"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="宋体"/>
-      <family val="3"/>
-      <charset val="134"/>
     </font>
     <font>
       <sz val="11"/>
@@ -600,7 +574,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -727,25 +701,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="87053440"/>
-        <c:axId val="87055360"/>
+        <c:axId val="99005184"/>
+        <c:axId val="99007104"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="87053440"/>
+        <c:axId val="99005184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87055360"/>
+        <c:crossAx val="99007104"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="87055360"/>
+        <c:axId val="99007104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -780,7 +754,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="87053440"/>
+        <c:crossAx val="99005184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -801,7 +775,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -903,25 +877,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="87083648"/>
-        <c:axId val="87237376"/>
+        <c:axId val="87496960"/>
+        <c:axId val="87523712"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="87083648"/>
+        <c:axId val="87496960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87237376"/>
+        <c:crossAx val="87523712"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="87237376"/>
+        <c:axId val="87523712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -949,7 +923,7 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87083648"/>
+        <c:crossAx val="87496960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -970,7 +944,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1328,8 +1302,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -1345,7 +1319,7 @@
   <sheetData>
     <row r="1" spans="1:13">
       <c r="A1" s="47" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B1" s="48"/>
       <c r="C1" s="48"/>
@@ -1470,10 +1444,10 @@
         <v>1</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C6" s="24" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D6" s="22"/>
       <c r="E6" s="22">
@@ -1507,10 +1481,10 @@
         <v>2</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D7" s="35"/>
       <c r="E7" s="35">
@@ -1544,10 +1518,10 @@
         <v>3</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D8" s="14"/>
       <c r="E8" s="35">
@@ -1581,10 +1555,10 @@
         <v>4</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D9" s="35"/>
       <c r="E9" s="35">
@@ -1615,10 +1589,10 @@
         <v>5</v>
       </c>
       <c r="B10" s="46" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="D10" s="35"/>
       <c r="E10" s="35">
@@ -1646,11 +1620,11 @@
     </row>
     <row r="11" spans="1:13" ht="18" customHeight="1">
       <c r="A11" s="38" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B11" s="11"/>
       <c r="C11" s="12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D11" s="33"/>
       <c r="E11" s="11"/>
@@ -1668,10 +1642,10 @@
         <v>6</v>
       </c>
       <c r="B12" s="28" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D12" s="34"/>
       <c r="E12" s="29">
@@ -1705,7 +1679,7 @@
         <v>5</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D13" s="35"/>
       <c r="E13" s="35">
@@ -1739,7 +1713,7 @@
         <v>5</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D14" s="35"/>
       <c r="E14" s="14">
@@ -1773,7 +1747,7 @@
         <v>5</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D15" s="35"/>
       <c r="E15" s="34">
@@ -1805,7 +1779,7 @@
       </c>
       <c r="B16" s="11"/>
       <c r="C16" s="12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D16" s="12"/>
       <c r="E16" s="11"/>
@@ -1823,10 +1797,10 @@
         <v>10</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D17" s="35"/>
       <c r="E17" s="35">
@@ -1863,7 +1837,7 @@
         <v>5</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D18" s="35"/>
       <c r="E18" s="35">
@@ -1900,7 +1874,7 @@
         <v>5</v>
       </c>
       <c r="C19" s="20" t="s">
-        <v>11</v>
+        <v>34</v>
       </c>
       <c r="D19" s="35"/>
       <c r="E19" s="35">
@@ -1934,7 +1908,7 @@
         <v>5</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D20" s="14"/>
       <c r="E20" s="35">
@@ -1968,7 +1942,7 @@
         <v>5</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D21" s="35"/>
       <c r="E21" s="14">
@@ -2060,7 +2034,7 @@
       </c>
       <c r="B26" s="11"/>
       <c r="C26" s="12" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D26" s="12"/>
       <c r="E26" s="11"/>
@@ -2079,7 +2053,7 @@
       </c>
       <c r="B27" s="16"/>
       <c r="C27" s="16" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D27" s="16"/>
       <c r="E27" s="17"/>
@@ -2173,7 +2147,7 @@
     </row>
     <row r="33" spans="3:10" ht="14.25">
       <c r="C33" s="49" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D33" s="49"/>
       <c r="E33" s="19">

</xml_diff>